<commit_message>
Ring Network & Zombie Network
</commit_message>
<xml_diff>
--- a/Manual/Config-ZH.xlsx
+++ b/Manual/Config-ZH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28110" windowHeight="13080"/>
+    <workbookView windowWidth="24210" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -278,9 +278,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -312,9 +312,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,15 +403,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,21 +423,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,67 +441,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -457,7 +457,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,7 +547,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,19 +559,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +589,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,13 +601,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,31 +619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,49 +631,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,6 +751,54 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -781,21 +829,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -804,39 +837,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -845,10 +845,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -857,10 +857,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -869,125 +869,125 @@
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,26 +1021,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1142,6 +1127,1362 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1213802</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4179570"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="-230505" y="1443990"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:ln/>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:ln/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2045335</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="3458845" y="1443990"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1212850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="-231140" y="4571365"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1825625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="8487410" y="1443990"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="6004560" y="1443990"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1136650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="矩形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="2550160" y="4876165"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="矩形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="6582410" y="5412740"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1290955" cy="4178935"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="矩形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18660000">
+          <a:off x="10367010" y="2606040"/>
+          <a:ext cx="4178935" cy="1290955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="t" anchorCtr="1">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>S-H4CK13</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="7200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1404,8 +2745,8 @@
   <sheetPr/>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1434,7 +2775,7 @@
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="21"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
@@ -1680,10 +3021,10 @@
       <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1703,10 +3044,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="6"/>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1726,10 +3067,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="6"/>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1749,10 +3090,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="6"/>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1774,10 +3115,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="6"/>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1797,10 +3138,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="6"/>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1820,10 +3161,10 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="6"/>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1843,10 +3184,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="6"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1870,7 +3211,7 @@
       <c r="A20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1893,7 +3234,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1916,7 +3257,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="6"/>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1939,7 +3280,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="6"/>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1964,7 +3305,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="6"/>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1987,10 +3328,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="6"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2010,10 +3351,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="6"/>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -2033,7 +3374,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="6"/>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2069,7 +3410,7 @@
       <c r="D28" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>65</v>
       </c>
       <c r="G28" s="9"/>
@@ -2103,13 +3444,13 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="G30" s="10"/>
       <c r="H30" s="7" t="s">
         <v>26</v>
@@ -2120,10 +3461,10 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="6" t="s">
         <v>3</v>
       </c>
@@ -2145,19 +3486,19 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G32" s="9"/>
@@ -2170,19 +3511,19 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="7" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="9"/>
@@ -2195,13 +3536,13 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="G34" s="10"/>
       <c r="H34" s="7" t="s">
         <v>26</v>
@@ -2212,10 +3553,10 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="16"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="6" t="s">
         <v>3</v>
       </c>
@@ -2225,40 +3566,40 @@
       <c r="E35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="18"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="13"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="16"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="6" t="s">
         <v>3</v>
       </c>
@@ -2270,32 +3611,32 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20" t="s">
+      <c r="B39" s="15"/>
+      <c r="C39" s="15" t="s">
         <v>82</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20" t="s">
+      <c r="B40" s="15"/>
+      <c r="C40" s="15" t="s">
         <v>84</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="20"/>
+      <c r="E40" s="15"/>
     </row>
   </sheetData>
   <sortState ref="B11:C18">
@@ -2436,5 +3777,6 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>